<commit_message>
[json] - [`assertEqual(expected,actual)`]: change the comparison logic and report format to improve accuracy and readability. The comparison now includes "objects of object" comparison.
[web]
- initial commit for browser-side performance metric collection logic. Not yet ready for prime time; only metrics collection for now.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_web_metrics.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_web_metrics.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D87445-3B7A-1440-8D10-933380A66D8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8432C7-1030-3C4E-ACD7-31DE7901B27F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19460" windowHeight="9840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26600" yWindow="860" windowWidth="24600" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>true</t>
   </si>
@@ -89,41 +90,95 @@
     <t>nexial.web.metrics.enabled</t>
   </si>
   <si>
+    <t>nexial.web.metrics.TTLB</t>
+  </si>
+  <si>
+    <t>site1.url</t>
+  </si>
+  <si>
+    <t>https://www.google.com</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.PageCompleteTime</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.Latency</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.DomInteractive</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.NetworkOverhead</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.FirstResponseTime</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.ContentDownload</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.PageReady</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.FirstInteractive</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.OnLoad</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.DomContentLoaded</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>// from PerformanceAPI -&gt; Navigation</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.BytesDownloaded</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.CachedResources</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.CompleteToLoad</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.CompressionRatio</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.DownloadToComplete</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.Fetched</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.FirstContentfulPaint</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.FirstPaint</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.InteractiveToComplete</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.PageDownloaded</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.ProcessingToInteractive</t>
+  </si>
+  <si>
+    <t>//nexial.web.metrics.RequestCount</t>
+  </si>
+  <si>
     <t>nexial.web.metrics.TTFB</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.TTLB</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.DownloadToComplete</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.PageDownloaded</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.InteractiveToComplete</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.ProcessingToInteractive</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.CompleteToLoad</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.RequestCount</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.BytesDownloaded</t>
-  </si>
-  <si>
-    <t>nexial.web.metrics.CachedResources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,16 +230,33 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -207,6 +279,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
@@ -219,7 +392,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -248,6 +421,50 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -630,15 +847,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA197"/>
+  <dimension ref="A1:AAA187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
     <col min="3" max="52" width="21.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="53" max="16384" width="10.7109375" style="2" collapsed="1"/>
@@ -679,34 +896,34 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="HA4" s="6"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="7"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="HA6" s="6"/>
       <c r="AAA6" s="7"/>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
@@ -716,7 +933,7 @@
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
@@ -724,7 +941,7 @@
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>0</v>
@@ -732,7 +949,7 @@
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>0</v>
@@ -740,7 +957,7 @@
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>0</v>
@@ -748,7 +965,7 @@
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>0</v>
@@ -756,7 +973,7 @@
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>0</v>
@@ -764,7 +981,7 @@
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -772,7 +989,7 @@
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -780,106 +997,198 @@
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="12"/>
+    </row>
+    <row r="34" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -1299,38 +1608,8 @@
     <row r="187" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="193" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="1"/>
-    </row>
-    <row r="194" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="1"/>
-    </row>
-    <row r="195" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="1"/>
-    </row>
-    <row r="196" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="1"/>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>

</xml_diff>

<commit_message>
[web] - [Browser Performance Metrics]: **NEW** feature in Nexial to capture browser performance metrics as part of Web automation. Collected data will be presented as HTML at the end of execution.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_web_metrics.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_web_metrics.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8432C7-1030-3C4E-ACD7-31DE7901B27F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EE9AC3-A319-E448-B567-87120452F996}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26600" yWindow="860" windowWidth="24600" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,6 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>true</t>
   </si>
@@ -129,9 +128,6 @@
     <t>nexial.web.metrics.DomContentLoaded</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>// from PerformanceAPI -&gt; Navigation</t>
   </si>
   <si>
@@ -172,13 +168,46 @@
   </si>
   <si>
     <t>nexial.web.metrics.TTFB</t>
+  </si>
+  <si>
+    <t>crypt:13b13cd4f92135972234e5e9c1bff7d4e0b36b4f1d84479b</t>
+  </si>
+  <si>
+    <t>ssh</t>
+  </si>
+  <si>
+    <t>site2.url</t>
+  </si>
+  <si>
+    <t>https://www.yahoo.com</t>
+  </si>
+  <si>
+    <t>searchTerm</t>
+  </si>
+  <si>
+    <t>Nexial Automation</t>
+  </si>
+  <si>
+    <t>site3.url</t>
+  </si>
+  <si>
+    <t>https://duckduckgo.com/</t>
+  </si>
+  <si>
+    <t>nexial.web.pageLoadWaitMs</t>
+  </si>
+  <si>
+    <t>nexial.web.highlight</t>
+  </si>
+  <si>
+    <t>80000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,6 +263,13 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -381,7 +417,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -391,8 +427,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -468,14 +507,19 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
@@ -847,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA187"/>
+  <dimension ref="A1:AAA192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -896,84 +940,94 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="HA4" s="6"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="7"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="HA6" s="6"/>
       <c r="AAA6" s="7"/>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="HA7" s="6"/>
       <c r="AAA7" s="7"/>
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="HA8" s="6"/>
+      <c r="AAA8" s="7"/>
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="HA9" s="6"/>
+      <c r="AAA9" s="7"/>
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="HA10" s="6"/>
+      <c r="AAA10" s="7"/>
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="HA11" s="6"/>
+      <c r="AAA11" s="7"/>
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="HA12" s="6"/>
+      <c r="AAA12" s="7"/>
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>0</v>
@@ -981,7 +1035,7 @@
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -989,7 +1043,7 @@
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -997,7 +1051,7 @@
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>0</v>
@@ -1005,7 +1059,7 @@
     </row>
     <row r="17" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>0</v>
@@ -1013,75 +1067,70 @@
     </row>
     <row r="18" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="8"/>
-    </row>
-    <row r="22" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="8"/>
+      <c r="B24" s="10" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>0</v>
-      </c>
+      <c r="A25" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="13"/>
       <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>0</v>
@@ -1090,7 +1139,7 @@
     </row>
     <row r="27" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>0</v>
@@ -1099,7 +1148,7 @@
     </row>
     <row r="28" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>0</v>
@@ -1108,7 +1157,7 @@
     </row>
     <row r="29" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>0</v>
@@ -1117,7 +1166,7 @@
     </row>
     <row r="30" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>0</v>
@@ -1126,69 +1175,103 @@
     </row>
     <row r="31" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="B36" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
-    </row>
-    <row r="34" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -1607,6 +1690,21 @@
     </row>
     <row r="187" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
+    </row>
+    <row r="188" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1"/>
+    </row>
+    <row r="190" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1"/>
+    </row>
+    <row r="191" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
@@ -1632,6 +1730,10 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{7DA8AD9F-24CA-7940-8549-94B6A4937F8D}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{A8BE0265-A1E0-2D43-ACCE-9097C5B35EC0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
[expression] - [JSON &raquo; keys(jsonpath)]: code fix to extract JSON keys correctly.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_web_metrics.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_web_metrics.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EE9AC3-A319-E448-B567-87120452F996}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3807A588-98B1-0D43-9B25-934DC081EAA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26600" yWindow="860" windowWidth="24600" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>true</t>
   </si>
@@ -131,42 +131,6 @@
     <t>// from PerformanceAPI -&gt; Navigation</t>
   </si>
   <si>
-    <t>//nexial.web.metrics.BytesDownloaded</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.CachedResources</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.CompleteToLoad</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.CompressionRatio</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.DownloadToComplete</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.Fetched</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.FirstContentfulPaint</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.FirstPaint</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.InteractiveToComplete</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.PageDownloaded</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.ProcessingToInteractive</t>
-  </si>
-  <si>
-    <t>//nexial.web.metrics.RequestCount</t>
-  </si>
-  <si>
     <t>nexial.web.metrics.TTFB</t>
   </si>
   <si>
@@ -201,6 +165,15 @@
   </si>
   <si>
     <t>80000</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.RequestCount</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.FirstContentfulPaint</t>
+  </si>
+  <si>
+    <t>nexial.web.metrics.FirstPaint</t>
   </si>
 </sst>
 </file>
@@ -292,7 +265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -326,19 +299,6 @@
       <bottom style="hair">
         <color theme="6" tint="0.39994506668294322"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </left>
-      <right style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </right>
-      <top style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -431,7 +391,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -475,35 +435,27 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -891,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA192"/>
+  <dimension ref="A1:AAA183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -947,17 +899,17 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="7"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -977,30 +929,30 @@
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="HA8" s="6"/>
       <c r="AAA8" s="7"/>
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="7"/>
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="HA10" s="6"/>
       <c r="AAA10" s="7"/>
@@ -1015,7 +967,7 @@
       <c r="HA11" s="6"/>
       <c r="AAA11" s="7"/>
     </row>
-    <row r="12" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:703" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1026,252 +978,210 @@
       <c r="AAA12" s="7"/>
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="8"/>
+      <c r="A30" s="1"/>
     </row>
     <row r="31" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="8"/>
+      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="8"/>
-    </row>
-    <row r="35" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="8"/>
-    </row>
-    <row r="36" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="1:3" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -1678,33 +1588,6 @@
     </row>
     <row r="183" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
-    </row>
-    <row r="184" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="1"/>
-    </row>
-    <row r="185" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="1"/>
-    </row>
-    <row r="186" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="187" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>

</xml_diff>